<commit_message>
added video presentation link in readme
</commit_message>
<xml_diff>
--- a/backend/data/water_usage_data.xlsx
+++ b/backend/data/water_usage_data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -63,6 +63,45 @@
   </si>
   <si>
     <t>518 liters</t>
+  </si>
+  <si>
+    <t>519 liters</t>
+  </si>
+  <si>
+    <t>520 liters</t>
+  </si>
+  <si>
+    <t>521 liters</t>
+  </si>
+  <si>
+    <t>522 liters</t>
+  </si>
+  <si>
+    <t>523 liters</t>
+  </si>
+  <si>
+    <t>524 liters</t>
+  </si>
+  <si>
+    <t>525 liters</t>
+  </si>
+  <si>
+    <t>526 liters</t>
+  </si>
+  <si>
+    <t>527 liters</t>
+  </si>
+  <si>
+    <t>528 liters</t>
+  </si>
+  <si>
+    <t>529 liters</t>
+  </si>
+  <si>
+    <t>530 liters</t>
+  </si>
+  <si>
+    <t>531 liters</t>
   </si>
 </sst>
 </file>
@@ -450,7 +489,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B37"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,6 +652,142 @@
         <v>16</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>